<commit_message>
[Pipette] 3개 type의 PCB 검토
</commit_message>
<xml_diff>
--- a/0_DOC/Plasma_Gen_Transformer_예상소모비용_20180203.xlsx
+++ b/0_DOC/Plasma_Gen_Transformer_예상소모비용_20180203.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -10,182 +10,198 @@
     <sheet name="전체 비용" sheetId="1" r:id="rId1"/>
     <sheet name="부품" sheetId="5" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="51">
+  <si>
+    <t>부품</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Item</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Description</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>MCU board Layout 설계비</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>PCB 제작비</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>MCU board PCB 제작비(SMT 비용 별도)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>SMT 비용</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>단가</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Comment</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>3일 x 250,000(일비)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>수량</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>전체비용</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Manual 납땜으로 작업(시험용)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>전체 비용</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>전체 소모비용</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>P_value</t>
+  </si>
+  <si>
+    <t>Q'ty</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Agency</t>
+  </si>
+  <si>
+    <t>MOQ</t>
+  </si>
+  <si>
+    <t>Cost[\]</t>
+  </si>
+  <si>
+    <t>MVG16VC220MF80</t>
+  </si>
+  <si>
+    <t>220uF 16V ALUMINUM CAPACITORS 6.3pi</t>
+  </si>
+  <si>
+    <t>ICbanQ</t>
+  </si>
+  <si>
+    <t>NTD5802N</t>
+  </si>
+  <si>
+    <t>Power MOSFET 40V, Single N-Channel, 101A DPAK</t>
+  </si>
+  <si>
+    <t>1.25mm 4-Pin SMD Straght 1A HEADER</t>
+  </si>
+  <si>
+    <t>TRANSFORMER CCFL 6W</t>
+  </si>
+  <si>
+    <t>CTX210607-R</t>
+  </si>
+  <si>
+    <t>TRANSFORMER CCFL 6W 13V 11MA SMD Turn-R:100</t>
+  </si>
+  <si>
+    <t>1.25mm 4-Pin Housing, Female</t>
+  </si>
+  <si>
+    <t>CRIMP TERMINAL 51021용 (1.25mm) AWG 28,30,32</t>
+  </si>
+  <si>
+    <t>구매수량</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Total</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>ICbanQ</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>53398-0471</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>CTX210605-R</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>CTX210609-R</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>51021-0400</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>50058-8000</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>부품 Total</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>부가세</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Transformer PCB 부품 비용</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>2층 높이 1.6mm(기본 10ea)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>부품 - 10ea 제작에 필요한 부품이며, Transformer는 3종 각2ea씩 구매이며, 특성 확인 후 재구매 예정</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
   <si>
     <t>PCB Layout</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>부품</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Item</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Description</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>MCU board Layout 설계비</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>PCB 제작비</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>MCU board PCB 제작비(SMT 비용 별도)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>SMT 비용</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>단가</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Comment</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>3일 x 250,000(일비)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>3set 제작</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>수량</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>전체비용</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Manual 납땜으로 작업(시험용)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>전체 비용</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>전체 소모비용</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>P_value</t>
-  </si>
-  <si>
-    <t>Q'ty</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Agency</t>
-  </si>
-  <si>
-    <t>MOQ</t>
-  </si>
-  <si>
-    <t>Cost[\]</t>
-  </si>
-  <si>
-    <t>MVG16VC220MF80</t>
-  </si>
-  <si>
-    <t>220uF 16V ALUMINUM CAPACITORS 6.3pi</t>
-  </si>
-  <si>
-    <t>ICbanQ</t>
-  </si>
-  <si>
-    <t>NTD5802N</t>
-  </si>
-  <si>
-    <t>Power MOSFET 40V, Single N-Channel, 101A DPAK</t>
-  </si>
-  <si>
-    <t>1.25mm 4-Pin SMD Straght 1A HEADER</t>
-  </si>
-  <si>
-    <t>TRANSFORMER CCFL 6W</t>
-  </si>
-  <si>
-    <t>CTX210607-R</t>
-  </si>
-  <si>
-    <t>TRANSFORMER CCFL 6W 13V 11MA SMD Turn-R:100</t>
-  </si>
-  <si>
-    <t>1.25mm 4-Pin Housing, Female</t>
-  </si>
-  <si>
-    <t>CRIMP TERMINAL 51021용 (1.25mm) AWG 28,30,32</t>
-  </si>
-  <si>
-    <t>구매수량</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Total</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>ICbanQ</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>53398-0471</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>CTX210605-R</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>CTX210609-R</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>51021-0400</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>50058-8000</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>부품 Total</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>부가세</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Transformer PCB 부품 비용</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>2층 높이 1.6mm(기본 10ea)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>부품 - 10ea 제작에 필요한 부품이며, Transformer는 3종 각2ea씩 구매이며, 특성 확인 후 재구매 예정</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>PCB Layout - 3개 Type으로 진행 ( 각 1일 )</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>NVMFS5C450NL</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>40V, 2.8mOhm , 110A, Single N−Channel Power MOSFET</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>부가세포함 총비용</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>10set 제작</t>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -196,12 +212,20 @@
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;?_-;_-@_-"/>
   </numFmts>
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -403,7 +427,7 @@
       <scheme val="major"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -587,6 +611,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -888,169 +918,169 @@
   </borders>
   <cellStyleXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0">
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="20" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="20" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1068,13 +1098,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1082,9 +1112,9 @@
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="41" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1107,8 +1137,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="55" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="55" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1117,53 +1147,65 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="55" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="55" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="55" applyFill="1" applyBorder="1"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="4" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="4" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="5" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="5" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="5" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="5" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="5" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="5" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="5" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="34" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="56">
@@ -1230,6 +1272,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1277,7 +1322,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1312,7 +1357,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1524,7 +1569,7 @@
   <dimension ref="B1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1539,74 +1584,72 @@
   <sheetData>
     <row r="1" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B1" s="21" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="14" t="s">
-        <v>3</v>
-      </c>
       <c r="D3" s="14" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E3" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="15" t="s">
         <v>8</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="15" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B4" s="7" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" s="8"/>
-      <c r="D4" s="16">
-        <v>10</v>
-      </c>
-      <c r="E4" s="46">
-        <v>12148</v>
-      </c>
+      <c r="D4" s="16"/>
+      <c r="E4" s="46"/>
       <c r="F4" s="17">
-        <f>D4*E4</f>
-        <v>121480</v>
-      </c>
-      <c r="G4" s="9"/>
+        <f>부품!I15</f>
+        <v>128744</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B5" s="10" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D5" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E5" s="11">
         <v>250000</v>
       </c>
       <c r="F5" s="11">
         <f>D5*E5</f>
-        <v>250000</v>
+        <v>750000</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B6" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>6</v>
       </c>
       <c r="D6" s="1">
         <v>1</v>
@@ -1619,15 +1662,15 @@
         <v>80000</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D7" s="5">
         <v>10</v>
@@ -1640,24 +1683,29 @@
         <v>100000</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>11</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="48" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="49"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="49"/>
+      <c r="B8" s="58" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="59"/>
+      <c r="D8" s="59"/>
+      <c r="E8" s="59"/>
       <c r="F8" s="19">
         <f>SUM(F4:F7)</f>
-        <v>551480</v>
+        <v>1058744</v>
       </c>
       <c r="G8" s="20"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1671,7 +1719,7 @@
   <mergeCells count="1">
     <mergeCell ref="B8:E8"/>
   </mergeCells>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1679,10 +1727,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:I14"/>
+  <dimension ref="B2:N21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1691,7 +1739,7 @@
     <col min="2" max="2" width="18.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="50.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5" style="59" customWidth="1"/>
+    <col min="5" max="5" width="9.5" style="57" customWidth="1"/>
     <col min="6" max="6" width="6.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.125" bestFit="1" customWidth="1"/>
@@ -1700,47 +1748,47 @@
   <sheetData>
     <row r="2" spans="2:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="21" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="2:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="49" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="51" t="s">
+      <c r="E3" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="F3" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="35" t="s">
+      <c r="G3" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="35" t="s">
+      <c r="H3" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" s="35" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B4" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="35" t="s">
+      <c r="C4" s="51">
+        <v>1</v>
+      </c>
+      <c r="D4" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="35" t="s">
+      <c r="E4" s="28" t="s">
         <v>34</v>
-      </c>
-      <c r="I3" s="35" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B4" s="52" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="53">
-        <v>1</v>
-      </c>
-      <c r="D4" s="54" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="28" t="s">
-        <v>36</v>
       </c>
       <c r="F4" s="28">
         <v>50</v>
@@ -1757,17 +1805,17 @@
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B5" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="56">
+      <c r="B5" s="53" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="54">
         <v>2</v>
       </c>
-      <c r="D5" s="57" t="s">
-        <v>27</v>
+      <c r="D5" s="55" t="s">
+        <v>25</v>
       </c>
       <c r="E5" s="33" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F5" s="33">
         <v>1</v>
@@ -1776,187 +1824,200 @@
         <v>1260</v>
       </c>
       <c r="H5" s="47">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="I5" s="38">
         <f>G5*H5</f>
-        <v>25200</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B6" s="55" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" s="56">
+        <v>12600</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="60" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="54">
+        <v>4</v>
+      </c>
+      <c r="D6" s="61" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="62" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="62">
         <v>1</v>
       </c>
-      <c r="D6" s="57" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="33">
-        <v>100</v>
-      </c>
-      <c r="G6" s="26">
-        <v>130</v>
-      </c>
-      <c r="H6" s="23">
-        <v>100</v>
+      <c r="G6" s="63">
+        <v>960</v>
+      </c>
+      <c r="H6" s="47">
+        <v>20</v>
       </c>
       <c r="I6" s="38">
         <f>G6*H6</f>
+        <v>19200</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B7" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="54">
+        <v>1</v>
+      </c>
+      <c r="D7" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="33">
+        <v>100</v>
+      </c>
+      <c r="G7" s="26">
+        <v>130</v>
+      </c>
+      <c r="H7" s="23">
+        <v>100</v>
+      </c>
+      <c r="I7" s="38">
+        <f>G7*H7</f>
         <v>13000</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B7" s="55" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7" s="56">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B8" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="54">
         <v>1</v>
       </c>
-      <c r="D7" s="57" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" s="33">
-        <v>1</v>
-      </c>
-      <c r="G7" s="26">
-        <v>7100</v>
-      </c>
-      <c r="H7" s="47">
-        <v>2</v>
-      </c>
-      <c r="I7" s="38">
-        <f t="shared" ref="I7:I10" si="0">G7*H7</f>
-        <v>14200</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B8" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="56">
-        <v>1</v>
-      </c>
-      <c r="D8" s="57" t="s">
-        <v>29</v>
+      <c r="D8" s="55" t="s">
+        <v>27</v>
       </c>
       <c r="E8" s="33" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F8" s="33">
         <v>1</v>
       </c>
       <c r="G8" s="26">
-        <v>10080</v>
+        <v>7100</v>
       </c>
       <c r="H8" s="47">
         <v>2</v>
       </c>
       <c r="I8" s="38">
+        <f t="shared" ref="I8:I11" si="0">G8*H8</f>
+        <v>14200</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B9" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="54">
+        <v>1</v>
+      </c>
+      <c r="D9" s="55" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="33">
+        <v>1</v>
+      </c>
+      <c r="G9" s="26">
+        <v>10080</v>
+      </c>
+      <c r="H9" s="47">
+        <v>2</v>
+      </c>
+      <c r="I9" s="38">
         <f t="shared" si="0"/>
         <v>20160</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B9" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="33">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B10" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="33">
         <v>1</v>
       </c>
-      <c r="D9" s="47" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" s="33">
+      <c r="D10" s="47" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="33">
         <v>1</v>
       </c>
-      <c r="G9" s="26">
+      <c r="G10" s="26">
         <v>11090</v>
       </c>
-      <c r="H9" s="47">
+      <c r="H10" s="47">
         <v>2</v>
       </c>
-      <c r="I9" s="38">
+      <c r="I10" s="38">
         <f t="shared" si="0"/>
         <v>22180</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B10" s="39" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" s="56">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B11" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="54">
         <v>1</v>
       </c>
-      <c r="D10" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="F10" s="33">
+      <c r="D11" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="33">
         <v>10</v>
       </c>
-      <c r="G10" s="26">
+      <c r="G11" s="26">
         <v>210</v>
       </c>
-      <c r="H10" s="47">
+      <c r="H11" s="47">
         <v>30</v>
       </c>
-      <c r="I10" s="38">
+      <c r="I11" s="38">
         <f t="shared" si="0"/>
         <v>6300</v>
       </c>
     </row>
-    <row r="11" spans="2:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="C11" s="58">
+    <row r="12" spans="2:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="56">
         <v>4</v>
       </c>
-      <c r="D11" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="F11" s="29">
+      <c r="D12" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="29">
         <v>100</v>
       </c>
-      <c r="G11" s="30">
+      <c r="G12" s="30">
         <v>20</v>
       </c>
-      <c r="H11" s="24">
+      <c r="H12" s="24">
         <v>220</v>
       </c>
-      <c r="I11" s="41">
-        <f>G11*H11</f>
+      <c r="I12" s="41">
+        <f>G12*H12</f>
         <v>4400</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B12" s="22"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="42" t="s">
-        <v>42</v>
-      </c>
-      <c r="I12" s="44">
-        <f>SUM(I4:I11)</f>
-        <v>110440</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.3">
@@ -1966,11 +2027,11 @@
       <c r="F13" s="22"/>
       <c r="G13" s="22"/>
       <c r="H13" s="42" t="s">
-        <v>43</v>
-      </c>
-      <c r="I13" s="45">
-        <f>I12*0.1</f>
-        <v>11044</v>
+        <v>40</v>
+      </c>
+      <c r="I13" s="44">
+        <f>SUM(I4:I12)</f>
+        <v>117040</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.3">
@@ -1978,17 +2039,38 @@
       <c r="C14" s="22"/>
       <c r="D14" s="22"/>
       <c r="F14" s="22"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="I14" s="46">
-        <f>I12+I13</f>
-        <v>121484</v>
-      </c>
+      <c r="G14" s="22"/>
+      <c r="H14" s="42" t="s">
+        <v>41</v>
+      </c>
+      <c r="I14" s="45">
+        <f>I13*0.1</f>
+        <v>11704</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="43" t="s">
+        <v>33</v>
+      </c>
+      <c r="I15" s="46">
+        <f>I13+I14</f>
+        <v>128744</v>
+      </c>
+    </row>
+    <row r="21" spans="10:14" x14ac:dyDescent="0.3">
+      <c r="J21" s="22"/>
+      <c r="K21" s="22"/>
+      <c r="L21" s="22"/>
+      <c r="M21" s="22"/>
+      <c r="N21" s="22"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[Pipette] Trans 부품 구매
</commit_message>
<xml_diff>
--- a/0_DOC/Plasma_Gen_Transformer_예상소모비용_20180203.xlsx
+++ b/0_DOC/Plasma_Gen_Transformer_예상소모비용_20180203.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="전체 비용" sheetId="1" r:id="rId1"/>
@@ -156,51 +156,51 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
+    <t>부품 Total</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>부가세</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Transformer PCB 부품 비용</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>2층 높이 1.6mm(기본 10ea)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>부품 - 10ea 제작에 필요한 부품이며, Transformer는 3종 각2ea씩 구매이며, 특성 확인 후 재구매 예정</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>PCB Layout</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>PCB Layout - 3개 Type으로 진행 ( 각 1일 )</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>NVMFS5C450NL</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>40V, 2.8mOhm , 110A, Single N−Channel Power MOSFET</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>부가세포함 총비용</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>10set 제작</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
     <t>50058-8000</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>부품 Total</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>부가세</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Transformer PCB 부품 비용</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>2층 높이 1.6mm(기본 10ea)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>부품 - 10ea 제작에 필요한 부품이며, Transformer는 3종 각2ea씩 구매이며, 특성 확인 후 재구매 예정</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>PCB Layout</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>PCB Layout - 3개 Type으로 진행 ( 각 1일 )</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>NVMFS5C450NL</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>40V, 2.8mOhm , 110A, Single N−Channel Power MOSFET</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>부가세포함 총비용</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>10set 제작</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -1189,23 +1189,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="5" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="34" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="5" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="34" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="56">
@@ -1568,7 +1568,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -1620,12 +1620,12 @@
         <v>128744</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B5" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>3</v>
@@ -1662,7 +1662,7 @@
         <v>80000</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -1683,16 +1683,16 @@
         <v>100000</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="58" t="s">
+      <c r="B8" s="62" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="59"/>
-      <c r="D8" s="59"/>
-      <c r="E8" s="59"/>
+      <c r="C8" s="63"/>
+      <c r="D8" s="63"/>
+      <c r="E8" s="63"/>
       <c r="F8" s="19">
         <f>SUM(F4:F7)</f>
         <v>1058744</v>
@@ -1701,12 +1701,12 @@
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="5:5" x14ac:dyDescent="0.3">
@@ -1729,8 +1729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:N21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1748,7 +1748,7 @@
   <sheetData>
     <row r="2" spans="2:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="2:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -1832,22 +1832,22 @@
       </c>
     </row>
     <row r="6" spans="2:9" s="22" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="60" t="s">
-        <v>47</v>
+      <c r="B6" s="58" t="s">
+        <v>46</v>
       </c>
       <c r="C6" s="54">
         <v>4</v>
       </c>
-      <c r="D6" s="61" t="s">
-        <v>48</v>
-      </c>
-      <c r="E6" s="62" t="s">
+      <c r="D6" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="60" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="62">
+      <c r="F6" s="60">
         <v>1</v>
       </c>
-      <c r="G6" s="63">
+      <c r="G6" s="61">
         <v>960</v>
       </c>
       <c r="H6" s="47">
@@ -1995,7 +1995,7 @@
     </row>
     <row r="12" spans="2:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="27" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="C12" s="56">
         <v>4</v>
@@ -2027,7 +2027,7 @@
       <c r="F13" s="22"/>
       <c r="G13" s="22"/>
       <c r="H13" s="42" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I13" s="44">
         <f>SUM(I4:I12)</f>
@@ -2041,7 +2041,7 @@
       <c r="F14" s="22"/>
       <c r="G14" s="22"/>
       <c r="H14" s="42" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I14" s="45">
         <f>I13*0.1</f>

</xml_diff>